<commit_message>
clean up example models and a test model
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_dry_model_with_mass_computation.xlsx
+++ b/tests/fixtures/test_dry_model_with_mass_computation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28700" windowHeight="13960" tabRatio="993"/>
+    <workbookView xWindow="-23940" yWindow="2780" windowWidth="31360" windowHeight="14660" tabRatio="993" firstSheet="5" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -21,64 +21,67 @@
     <sheet name="!!Species types" sheetId="7" r:id="rId7"/>
     <sheet name="!!Species" sheetId="8" r:id="rId8"/>
     <sheet name="!!Initial species concentration" sheetId="9" r:id="rId9"/>
-    <sheet name="!!Observables" sheetId="10" r:id="rId10"/>
-    <sheet name="!!Functions" sheetId="11" r:id="rId11"/>
-    <sheet name="!!Reactions" sheetId="12" r:id="rId12"/>
-    <sheet name="!!Rate laws" sheetId="13" r:id="rId13"/>
-    <sheet name="!!dFBA objectives" sheetId="14" r:id="rId14"/>
-    <sheet name="!!dFBA objective reactions" sheetId="15" r:id="rId15"/>
-    <sheet name="!!dFBA objective species" sheetId="16" r:id="rId16"/>
-    <sheet name="!!Parameters" sheetId="17" r:id="rId17"/>
-    <sheet name="!!Stop conditions" sheetId="18" r:id="rId18"/>
-    <sheet name="!!Observations" sheetId="19" r:id="rId19"/>
-    <sheet name="!!Observation sets" sheetId="20" r:id="rId20"/>
-    <sheet name="!!Conclusions" sheetId="21" r:id="rId21"/>
-    <sheet name="!!References" sheetId="22" r:id="rId22"/>
-    <sheet name="!!Authors" sheetId="23" r:id="rId23"/>
-    <sheet name="!!Changes" sheetId="24" r:id="rId24"/>
+    <sheet name="Compartment mass computation" sheetId="25" r:id="rId10"/>
+    <sheet name="!!Observables" sheetId="10" r:id="rId11"/>
+    <sheet name="!!Functions" sheetId="11" r:id="rId12"/>
+    <sheet name="!!Reactions" sheetId="12" r:id="rId13"/>
+    <sheet name="!!Rate laws" sheetId="13" r:id="rId14"/>
+    <sheet name="!!dFBA objectives" sheetId="14" r:id="rId15"/>
+    <sheet name="!!dFBA objective reactions" sheetId="15" r:id="rId16"/>
+    <sheet name="!!dFBA objective species" sheetId="16" r:id="rId17"/>
+    <sheet name="!!Parameters" sheetId="17" r:id="rId18"/>
+    <sheet name="!!Stop conditions" sheetId="18" r:id="rId19"/>
+    <sheet name="!!Observations" sheetId="19" r:id="rId20"/>
+    <sheet name="!!Observation sets" sheetId="20" r:id="rId21"/>
+    <sheet name="!!Conclusions" sheetId="21" r:id="rId22"/>
+    <sheet name="!!References" sheetId="22" r:id="rId23"/>
+    <sheet name="!!Authors" sheetId="23" r:id="rId24"/>
+    <sheet name="!!Changes" sheetId="24" r:id="rId25"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId25"/>
     <externalReference r:id="rId26"/>
     <externalReference r:id="rId27"/>
     <externalReference r:id="rId28"/>
     <externalReference r:id="rId29"/>
+    <externalReference r:id="rId30"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'!!_Table of contents'!$A$1:$C$24</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'!!Compartments'!$A$2:$G$4</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">'!!Parameters'!$A$1:$F$11</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'!!Reactions'!$A$2:$D$6</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">'!!References'!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">'!!Parameters'!$A$1:$F$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'!!Reactions'!$A$2:$D$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="22" hidden="1">'!!References'!$A$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'!!Species types'!$A$2:$K$8</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="5">[1]Compartments!$A$2:$G$4</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="16">[4]Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="11">[3]Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="21">[5]References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0" localSheetId="6">'[2]Species types'!$A$2:$K$7</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="17">[2]Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="12">[3]Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="22">[4]References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="6">'[5]Species types'!$A$2:$K$7</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="5">[1]Compartments!$A$2:$G$4</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="16">[4]Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="11">[3]Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="21">[5]References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0" localSheetId="6">'[2]Species types'!$A$2:$K$7</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="17">[2]Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="12">[3]Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="22">[4]References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="6">'[5]Species types'!$A$2:$K$7</definedName>
     <definedName name="_FilterDatabase_0_0_0" localSheetId="5">[1]Compartments!$A$2:$G$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="16">[4]Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="11">[3]Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="21">[5]References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0" localSheetId="6">'[2]Species types'!$A$2:$K$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="17">[2]Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="12">[3]Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="22">[4]References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0" localSheetId="6">'[5]Species types'!$A$2:$K$7</definedName>
     <definedName name="_FilterDatabase_0_0_0_0" localSheetId="5">[1]Compartments!$A$2:$G$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="16">[4]Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="11">[3]Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="21">[5]References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="6">'[2]Species types'!$A$2:$K$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="17">[2]Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="12">[3]Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="22">[4]References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0" localSheetId="6">'[5]Species types'!$A$2:$K$7</definedName>
     <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="5">[1]Compartments!$A$2:$G$4</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="16">[4]Parameters!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="11">[3]Reactions!$A$2:$D$6</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="21">[5]References!$A$1:$D$1</definedName>
-    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="6">'[2]Species types'!$A$2:$K$7</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="17">[2]Parameters!$A$1:$F$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="12">[3]Reactions!$A$2:$D$6</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="22">[4]References!$A$1:$D$1</definedName>
+    <definedName name="_FilterDatabase_0_0_0_0_0" localSheetId="6">'[5]Species types'!$A$2:$K$7</definedName>
+    <definedName name="fractionDryWeight">'!!Parameters'!$D$3</definedName>
+    <definedName name="volume_c">'!!Compartments'!$I$4</definedName>
+    <definedName name="volume_e">'!!Compartments'!$I$5</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -91,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="281">
   <si>
     <t>!!!ObjTables ObjTablesVersion='0.0.8'</t>
   </si>
@@ -501,15 +504,6 @@
     <t>!Species</t>
   </si>
   <si>
-    <t>!Compartment volume</t>
-  </si>
-  <si>
-    <t>!Mass</t>
-  </si>
-  <si>
-    <t>!Dry weight</t>
-  </si>
-  <si>
     <t>dist-init-conc-specie_2[c]</t>
   </si>
   <si>
@@ -928,6 +922,21 @@
   </si>
   <si>
     <t>!Intention type</t>
+  </si>
+  <si>
+    <t>Compartment volume</t>
+  </si>
+  <si>
+    <t>Molecular weight</t>
+  </si>
+  <si>
+    <t>Mass</t>
+  </si>
+  <si>
+    <t>Dry weight</t>
+  </si>
+  <si>
+    <t>Compartment</t>
   </si>
 </sst>
 </file>
@@ -1040,7 +1049,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1113,6 +1122,9 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1163,7 +1175,7 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Species types"/>
+      <sheetName val="Parameters"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
@@ -1189,7 +1201,7 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Parameters"/>
+      <sheetName val="References"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
@@ -1202,7 +1214,7 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="References"/>
+      <sheetName val="Species types"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
@@ -1471,7 +1483,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A19" sqref="A19:A21"/>
     </sheetView>
@@ -1743,13 +1755,205 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:L11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="A4" sqref="A4:XFD5"/>
+      <selection pane="topRight" activeCell="A4" sqref="A4:XFD5"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4:XFD5"/>
+      <selection pane="bottomRight" activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.83203125" style="25" customWidth="1"/>
+    <col min="2" max="2" width="20" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" style="25" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="25" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" style="25" customWidth="1"/>
+    <col min="6" max="1013" width="8.83203125" style="25" customWidth="1"/>
+    <col min="1014" max="1014" width="9" style="25" customWidth="1"/>
+    <col min="1015" max="16384" width="9" style="25"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>276</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="A3" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="4">
+        <f>volume_c</f>
+        <v>4.58E-17</v>
+      </c>
+      <c r="C3" s="25">
+        <f>'!!Species types'!G5</f>
+        <v>2</v>
+      </c>
+      <c r="D3" s="23">
+        <f>C3*B3</f>
+        <v>9.1599999999999999E-17</v>
+      </c>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="A4" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="4">
+        <f>volume_c</f>
+        <v>4.58E-17</v>
+      </c>
+      <c r="C4" s="25">
+        <f>'!!Species types'!G7</f>
+        <v>4</v>
+      </c>
+      <c r="D4" s="23">
+        <f t="shared" ref="D4:D9" si="0">C3*B3</f>
+        <v>9.1599999999999999E-17</v>
+      </c>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="A5" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="4">
+        <f>volume_c</f>
+        <v>4.58E-17</v>
+      </c>
+      <c r="C5" s="25">
+        <f>'!!Species types'!G8</f>
+        <v>5</v>
+      </c>
+      <c r="D5" s="23">
+        <f t="shared" si="0"/>
+        <v>1.832E-16</v>
+      </c>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="A6" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="4">
+        <f>volume_c</f>
+        <v>4.58E-17</v>
+      </c>
+      <c r="C6" s="25">
+        <f>'!!Species types'!G9</f>
+        <v>6</v>
+      </c>
+      <c r="D6" s="23">
+        <f t="shared" si="0"/>
+        <v>2.2899999999999997E-16</v>
+      </c>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="A7" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" s="4">
+        <f>volume_e</f>
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="C7" s="25">
+        <f>'!!Species types'!G4</f>
+        <v>1</v>
+      </c>
+      <c r="D7" s="23">
+        <f t="shared" si="0"/>
+        <v>2.748E-16</v>
+      </c>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" s="4">
+        <f>volume_e</f>
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="C8" s="25">
+        <f>'!!Species types'!G5</f>
+        <v>2</v>
+      </c>
+      <c r="D8" s="23">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="D9" s="23">
+        <f>SUMIF(A$2:A$7,"c",D$2:D$7)</f>
+        <v>5.9539999999999997E-16</v>
+      </c>
+      <c r="E9" s="4">
+        <f>D8*fractionDryWeight</f>
+        <v>2.9999999999999998E-13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="D10" s="23">
+        <f>SUMIF(A$2:A$7,"e",D$2:D$7)</f>
+        <v>2.748E-16</v>
+      </c>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="D11" s="23">
+        <f>SUBTOTAL(9,D2:D7)</f>
+        <v>8.7020000000000002E-16</v>
+      </c>
+      <c r="E11" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
+      <selection activeCell="A4" sqref="A4:XFD5"/>
+      <selection pane="topRight" activeCell="A4" sqref="A4:XFD5"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4:XFD5"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1761,7 +1965,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1772,7 +1976,7 @@
         <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>82</v>
@@ -1799,15 +2003,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
+      <selection activeCell="A4" sqref="A4:XFD5"/>
+      <selection pane="topRight" activeCell="A4" sqref="A4:XFD5"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4:XFD5"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1819,10 +2024,10 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="28" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>29</v>
       </c>
@@ -1830,7 +2035,7 @@
         <v>31</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>82</v>
@@ -1853,11 +2058,11 @@
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="9" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>92</v>
@@ -1865,11 +2070,11 @@
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="9" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>92</v>
@@ -1881,15 +2086,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMM7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
+      <selection activeCell="A4" sqref="A4:XFD5"/>
+      <selection pane="topRight" activeCell="A4" sqref="A4:XFD5"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4:XFD5"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1905,7 +2111,7 @@
   <sheetData>
     <row r="1" spans="1:1027" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:1027" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -1915,11 +2121,11 @@
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
-      <c r="G2" s="27" t="s">
-        <v>157</v>
-      </c>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
+      <c r="G2" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
       <c r="J2" s="9"/>
       <c r="K2" s="9"/>
       <c r="L2" s="9"/>
@@ -2947,22 +3153,22 @@
         <v>31</v>
       </c>
       <c r="C3" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="F3" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="G3" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="H3" s="14" t="s">
         <v>160</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>161</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>163</v>
       </c>
       <c r="I3" s="14" t="s">
         <v>82</v>
@@ -3998,22 +4204,22 @@
     </row>
     <row r="4" spans="1:1027" ht="28" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>64</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E4" s="11">
         <v>0</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G4" s="11">
         <v>0</v>
@@ -4022,28 +4228,28 @@
         <v>1</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="J4" s="24"/>
     </row>
     <row r="5" spans="1:1027" ht="28" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>64</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E5" s="11">
         <v>1</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
@@ -4052,22 +4258,22 @@
     </row>
     <row r="6" spans="1:1027" ht="28" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C6" s="19" t="s">
         <v>68</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E6" s="11">
         <v>1</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
@@ -4076,22 +4282,22 @@
     </row>
     <row r="7" spans="1:1027" ht="28" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C7" s="19" t="s">
         <v>68</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E7" s="11">
         <v>0</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
@@ -4108,7 +4314,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M7"/>
   <sheetViews>
@@ -4133,7 +4339,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -4144,16 +4350,16 @@
         <v>31</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>108</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G2" s="14" t="s">
         <v>82</v>
@@ -4176,88 +4382,88 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C3" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="G3" s="19" t="s">
         <v>164</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>183</v>
-      </c>
-      <c r="G3" s="19" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="F4" s="19" t="s">
         <v>182</v>
       </c>
-      <c r="F4" s="19" t="s">
-        <v>185</v>
-      </c>
       <c r="G4" s="19" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="M6" s="4"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="M7" s="4"/>
     </row>
@@ -4267,7 +4473,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L3"/>
   <sheetViews>
@@ -4286,7 +4492,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -4297,19 +4503,19 @@
         <v>31</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>82</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="H2" s="14" t="s">
         <v>44</v>
@@ -4329,19 +4535,19 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C3" s="19" t="s">
         <v>64</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E3" s="19" t="s">
         <v>94</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G3" s="19" t="s">
         <v>43</v>
@@ -4352,7 +4558,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
@@ -4373,7 +4579,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -4384,13 +4590,13 @@
         <v>31</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>82</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F2" s="14" t="s">
         <v>44</v>
@@ -4410,22 +4616,22 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>197</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>200</v>
       </c>
       <c r="C3" s="19" t="s">
         <v>64</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>92</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -4434,7 +4640,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K6"/>
   <sheetViews>
@@ -4457,7 +4663,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -4468,7 +4674,7 @@
         <v>31</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>135</v>
@@ -4497,13 +4703,13 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D3" s="19" t="s">
         <v>125</v>
@@ -4512,21 +4718,21 @@
         <v>-3</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D4" s="19" t="s">
         <v>127</v>
@@ -4535,18 +4741,18 @@
         <v>-4</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D5" s="19" t="s">
         <v>128</v>
@@ -4555,18 +4761,18 @@
         <v>1</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>129</v>
@@ -4575,7 +4781,7 @@
         <v>2</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -4584,7 +4790,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
@@ -4592,22 +4798,25 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="8.83203125" style="19" customWidth="1"/>
-    <col min="4" max="4" width="9.1640625" style="19" customWidth="1"/>
-    <col min="5" max="9" width="8.83203125" style="19" customWidth="1"/>
-    <col min="10" max="1026" width="8.83203125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="12.5" style="19" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="19" customWidth="1"/>
+    <col min="6" max="6" width="24.6640625" style="19" customWidth="1"/>
+    <col min="7" max="9" width="8.83203125" style="19" customWidth="1"/>
+    <col min="10" max="10" width="20.5" style="8" customWidth="1"/>
+    <col min="11" max="1026" width="8.83203125" style="8" customWidth="1"/>
     <col min="1027" max="1027" width="9" style="8" customWidth="1"/>
     <col min="1028" max="16384" width="9" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -4624,7 +4833,7 @@
         <v>102</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F2" s="14" t="s">
         <v>82</v>
@@ -4647,114 +4856,114 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D3" s="19">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="F3" s="19" t="s">
         <v>94</v>
       </c>
       <c r="J3" s="19" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D4" s="19">
         <v>1</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D5" s="4">
         <v>2000</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D6" s="4">
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D7" s="4">
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D8" s="4">
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D9" s="4">
         <v>1E-3</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D10" s="4">
         <v>6.02214075862E+23</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -4765,7 +4974,7 @@
         <v>1100</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -4776,7 +4985,7 @@
         <v>1000</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -4786,7 +4995,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -4806,7 +5015,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -4817,7 +5026,7 @@
         <v>31</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>82</v>
@@ -4841,132 +5050,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="V1" sqref="V1:V1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="9" style="19" customWidth="1"/>
-    <col min="2" max="16384" width="9" style="19"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G2" s="29" t="s">
-        <v>232</v>
-      </c>
-      <c r="H2" s="26"/>
-      <c r="I2" s="29" t="s">
-        <v>233</v>
-      </c>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="Q2" s="30" t="s">
-        <v>234</v>
-      </c>
-      <c r="R2" s="26"/>
-      <c r="S2" s="30" t="s">
-        <v>235</v>
-      </c>
-      <c r="T2" s="26"/>
-    </row>
-    <row r="3" spans="1:23" ht="42" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:N2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="S2:T2"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -5086,6 +5169,132 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="V1" sqref="V1:V1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9" style="19" customWidth="1"/>
+    <col min="2" max="16384" width="9" style="19"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G2" s="30" t="s">
+        <v>229</v>
+      </c>
+      <c r="H2" s="27"/>
+      <c r="I2" s="30" t="s">
+        <v>230</v>
+      </c>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="Q2" s="31" t="s">
+        <v>231</v>
+      </c>
+      <c r="R2" s="27"/>
+      <c r="S2" s="31" t="s">
+        <v>232</v>
+      </c>
+      <c r="T2" s="27"/>
+    </row>
+    <row r="3" spans="1:23" ht="42" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5105,7 +5314,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5116,7 +5325,7 @@
         <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>44</v>
@@ -5145,7 +5354,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N11"/>
   <sheetViews>
@@ -5166,14 +5375,14 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G2" s="30" t="s">
-        <v>246</v>
-      </c>
-      <c r="H2" s="26"/>
+      <c r="G2" s="31" t="s">
+        <v>243</v>
+      </c>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -5186,7 +5395,7 @@
         <v>102</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>82</v>
@@ -5213,10 +5422,10 @@
         <v>54</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5264,7 +5473,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R2"/>
   <sheetViews>
@@ -5282,7 +5491,7 @@
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
@@ -5293,46 +5502,46 @@
         <v>31</v>
       </c>
       <c r="C2" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>248</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="F2" s="14" t="s">
         <v>250</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>251</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>252</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>253</v>
       </c>
       <c r="G2" s="14" t="s">
         <v>108</v>
       </c>
       <c r="H2" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>252</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="K2" s="14" t="s">
         <v>254</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="L2" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="M2" s="14" t="s">
         <v>256</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="N2" s="14" t="s">
         <v>257</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="O2" s="14" t="s">
         <v>258</v>
       </c>
-      <c r="M2" s="14" t="s">
+      <c r="P2" s="14" t="s">
         <v>259</v>
-      </c>
-      <c r="N2" s="14" t="s">
-        <v>260</v>
-      </c>
-      <c r="O2" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="P2" s="14" t="s">
-        <v>262</v>
       </c>
       <c r="Q2" s="14" t="s">
         <v>44</v>
@@ -5348,7 +5557,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
@@ -5367,7 +5576,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -5378,28 +5587,28 @@
         <v>31</v>
       </c>
       <c r="C2" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="G2" s="14" t="s">
         <v>264</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="H2" s="14" t="s">
         <v>265</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="I2" s="14" t="s">
         <v>266</v>
       </c>
-      <c r="F2" s="14" t="s">
-        <v>250</v>
-      </c>
-      <c r="G2" s="14" t="s">
+      <c r="J2" s="14" t="s">
         <v>267</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>268</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="J2" s="14" t="s">
-        <v>270</v>
       </c>
       <c r="K2" s="14" t="s">
         <v>44</v>
@@ -5413,7 +5622,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
@@ -5432,7 +5641,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -5446,25 +5655,25 @@
         <v>108</v>
       </c>
       <c r="D2" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>270</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="G2" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="H2" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="I2" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="J2" s="14" t="s">
         <v>275</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>276</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>277</v>
-      </c>
-      <c r="J2" s="14" t="s">
-        <v>278</v>
       </c>
       <c r="K2" s="14" t="s">
         <v>44</v>
@@ -5482,10 +5691,10 @@
         <v>54</v>
       </c>
       <c r="P2" s="14" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="Q2" s="14" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -5719,18 +5928,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMR5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M4" sqref="M4"/>
+      <selection pane="bottomRight" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="9" width="8.83203125" style="19" customWidth="1"/>
     <col min="10" max="10" width="9.33203125" style="19" customWidth="1"/>
-    <col min="11" max="1035" width="8.83203125" style="19" customWidth="1"/>
+    <col min="11" max="19" width="8.83203125" style="19" customWidth="1"/>
+    <col min="20" max="20" width="43.83203125" style="19" customWidth="1"/>
+    <col min="21" max="1035" width="8.83203125" style="19" customWidth="1"/>
     <col min="1036" max="1036" width="9" style="19" customWidth="1"/>
     <col min="1037" max="16384" width="9" style="19"/>
   </cols>
@@ -5748,19 +5959,19 @@
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
       <c r="L2" s="9"/>
-      <c r="M2" s="25" t="s">
+      <c r="M2" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
       <c r="Q2" s="9"/>
       <c r="R2" s="9"/>
       <c r="S2" s="9"/>
@@ -7854,7 +8065,7 @@
       <c r="AMQ3" s="9"/>
       <c r="AMR3" s="9"/>
     </row>
-    <row r="4" spans="1:1032" ht="252" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1032" ht="42" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
         <v>84</v>
       </c>
@@ -7907,7 +8118,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:1032" ht="168" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1032" ht="42" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
         <v>89</v>
       </c>
@@ -7972,11 +8183,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F3" sqref="F3:F8"/>
+      <selection activeCell="A4" sqref="A4:XFD5"/>
+      <selection pane="topRight" activeCell="A4" sqref="A4:XFD5"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4:XFD5"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7996,14 +8208,14 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -8176,11 +8388,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
+      <selection activeCell="A4" sqref="A4:XFD5"/>
+      <selection pane="topRight" activeCell="A4" sqref="A4:XFD5"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4:XFD5"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8352,13 +8565,14 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D2" sqref="D2:D7"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="A4" sqref="A4:XFD5"/>
+      <selection pane="topRight" activeCell="A4" sqref="A4:XFD5"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4:XFD5"/>
+      <selection pane="bottomRight" activeCell="N1" sqref="N1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
@@ -8366,22 +8580,21 @@
     <col min="1" max="1" width="21" style="19" customWidth="1"/>
     <col min="2" max="2" width="8.83203125" style="19" customWidth="1"/>
     <col min="3" max="3" width="10" style="19" customWidth="1"/>
-    <col min="4" max="4" width="11" style="19" customWidth="1"/>
+    <col min="4" max="4" width="16.5" style="19" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.6640625" style="19" customWidth="1"/>
-    <col min="6" max="16" width="8.83203125" style="19" customWidth="1"/>
-    <col min="17" max="17" width="10.1640625" style="19" customWidth="1"/>
-    <col min="18" max="18" width="9.1640625" style="19" customWidth="1"/>
-    <col min="19" max="1026" width="8.83203125" style="19" customWidth="1"/>
-    <col min="1027" max="1027" width="9" style="19" customWidth="1"/>
-    <col min="1028" max="16384" width="9" style="19"/>
+    <col min="6" max="7" width="8.83203125" style="19" customWidth="1"/>
+    <col min="8" max="12" width="8.83203125" style="19" hidden="1" customWidth="1"/>
+    <col min="13" max="1021" width="8.83203125" style="19" customWidth="1"/>
+    <col min="1022" max="1022" width="9" style="19" customWidth="1"/>
+    <col min="1023" max="16384" width="9" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:18" outlineLevel="2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>29</v>
       </c>
@@ -8418,25 +8631,10 @@
       <c r="L2" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="N2" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="O2" s="14" t="s">
+    </row>
+    <row r="3" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="A3" s="19" t="s">
         <v>136</v>
-      </c>
-      <c r="P2" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q2" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="R2" s="14" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" outlineLevel="2" x14ac:dyDescent="0.2">
-      <c r="A3" s="19" t="s">
-        <v>139</v>
       </c>
       <c r="C3" s="19" t="s">
         <v>127</v>
@@ -8448,28 +8646,12 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="N3" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="O3" s="4" t="e">
-        <f>VLOOKUP(N2,[1]Compartments!A:I,9,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P3" s="19" t="e">
-        <f>'[2]Species types'!G4</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q3" s="23" t="e">
-        <f t="shared" ref="Q3:Q8" si="0">P2*O2</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R3" s="4"/>
-    </row>
-    <row r="4" spans="1:18" outlineLevel="2" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>129</v>
@@ -8481,28 +8663,12 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="N4" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="O4" s="4" t="e">
-        <f>VLOOKUP(N3,[1]Compartments!A:I,9,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P4" s="19" t="e">
-        <f>'[2]Species types'!G6</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q4" s="23" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="R4" s="4"/>
-    </row>
-    <row r="5" spans="1:18" outlineLevel="2" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>130</v>
@@ -8514,28 +8680,12 @@
         <v>1E-3</v>
       </c>
       <c r="G5" s="23" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.2">
+      <c r="A6" s="19" t="s">
         <v>140</v>
-      </c>
-      <c r="N5" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="O5" s="4" t="e">
-        <f>VLOOKUP(N4,[1]Compartments!A:I,9,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P5" s="19" t="e">
-        <f>'[2]Species types'!G7</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q5" s="23" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="R5" s="4"/>
-    </row>
-    <row r="6" spans="1:18" outlineLevel="2" x14ac:dyDescent="0.2">
-      <c r="A6" s="19" t="s">
-        <v>143</v>
       </c>
       <c r="C6" s="19" t="s">
         <v>131</v>
@@ -8547,27 +8697,12 @@
         <v>2E-3</v>
       </c>
       <c r="G6" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="N6" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="O6" s="4" t="e">
-        <f>VLOOKUP(N5,[1]Compartments!A:I,9,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P6" s="19">
-        <v>6</v>
-      </c>
-      <c r="Q6" s="23" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="R6" s="4"/>
-    </row>
-    <row r="7" spans="1:18" outlineLevel="2" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C7" s="19" t="s">
         <v>132</v>
@@ -8579,28 +8714,12 @@
         <v>1.4799999999999999E-4</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="N7" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="O7" s="4" t="e">
-        <f>VLOOKUP(N6,[1]Compartments!A:I,9,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P7" s="19" t="e">
-        <f>'[2]Species types'!G3</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q7" s="23" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R7" s="4"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C8" s="19" t="s">
         <v>133</v>
@@ -8612,60 +8731,8 @@
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="N8" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="O8" s="4" t="e">
-        <f>VLOOKUP(N7,[1]Compartments!A:I,9,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P8" s="19" t="e">
-        <f>'[2]Species types'!G4</f>
-        <v>#REF!</v>
-      </c>
-      <c r="Q8" s="23" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-      <c r="R8" s="4"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="N9" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="O9" s="4"/>
-      <c r="Q9" s="23" t="e">
-        <f>SUMIF(N$2:N$7,"c",Q$2:Q$7)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R9" s="4" t="e">
-        <f>Q8*[4]Parameters!D2</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="N10" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="O10" s="4"/>
-      <c r="Q10" s="23" t="e">
-        <f>SUMIF(N$2:N$7,"e",Q$2:Q$7)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R10" s="4"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="N11" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="O11" s="4"/>
-      <c r="Q11" s="23" t="e">
-        <f>SUBTOTAL(9,Q2:Q7)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R11" s="4"/>
+        <v>137</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>